<commit_message>
added details adn corrected mistakes in web scrapper/ README.MD
</commit_message>
<xml_diff>
--- a/Web Scrapper/Skill Frequency.xlsx
+++ b/Web Scrapper/Skill Frequency.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>3Ds Max</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IT Skills</t>
+          <t>Maya</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AWS</t>
+          <t>Photoshop</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Java</t>
+          <t>Cinema 4D</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -503,11 +503,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Django</t>
+          <t>Design</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cloud</t>
+          <t>3D Design</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>JavaScript</t>
+          <t>3D Compositing</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -542,7 +542,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Azure</t>
+          <t>Simulation Artist</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -555,7 +555,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Houdini</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Machine Learning</t>
+          <t>FX Artist</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Big Data</t>
+          <t>Fume FX</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -594,7 +594,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hive</t>
+          <t>Time Management</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EC2</t>
+          <t>Technical Skills</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>REST services</t>
+          <t>Particle Simulation</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>RPC</t>
+          <t>3D Generalist</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Java scripts</t>
+          <t>texturing</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>JQuery</t>
+          <t>3D Modeler</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>REST</t>
+          <t>Mudbox</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Machine learning</t>
+          <t>Rigging</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Agile methodologies</t>
+          <t>3D max</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>CorelDraw</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NLP</t>
+          <t>Visual Designer</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Rabbitmq</t>
+          <t>2D Design</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Celery</t>
+          <t>Visualiser</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Docker</t>
+          <t>Sketchup</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Illustrator</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SQL</t>
+          <t>AutoCAD</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SNS</t>
+          <t>Texturing</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ETL</t>
+          <t>Interiors</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Apache</t>
+          <t>Sewing</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CSS</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Angular</t>
+          <t>Visual Effects</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>HTML</t>
+          <t>VRAY</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Html5</t>
+          <t>3D Character Animation</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Python Programming</t>
+          <t>Art</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -906,11 +906,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Communication</t>
+          <t>Unity3D</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>3D Maya</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Mako</t>
+          <t>Lumion</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Jinja</t>
+          <t>Google Sketchup</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Flask</t>
+          <t>REVIT</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Snowflake</t>
+          <t>Execution</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RDS</t>
+          <t>Project Management</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>communication</t>
+          <t>Rendering</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>troubleshooting</t>
+          <t>Lighting</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>New Product</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Git</t>
+          <t>3D Modeling</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>automation frameworks</t>
+          <t>Project Coordination</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Bugzilla</t>
+          <t>Lead Generation</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>C programming</t>
+          <t>Project Sales</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Javascript</t>
+          <t>Bdm</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>Business Development Management</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SQS</t>
+          <t>VAVE</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>written communication</t>
+          <t>3D Cad</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>AJAX</t>
+          <t>UG NX</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>XML</t>
+          <t>Teamcenter</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Statistical programming</t>
+          <t>Graphics</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Networking</t>
+          <t>3D</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Data management</t>
+          <t>Kaizen</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Access management</t>
+          <t>Time management</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>devops</t>
+          <t>Venture capital</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Informatica</t>
+          <t>Architecture</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SDK</t>
+          <t>Adobe Premiere Pro</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Vulnerability management</t>
+          <t>VFX</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Fullstack Developer</t>
+          <t>Adobe After Effects</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>React</t>
+          <t>Compositing</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DevOps</t>
+          <t>3D Graphics</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Jenkins</t>
+          <t>UX</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Application Management</t>
+          <t>3D Animation</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1335,140 +1335,10 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>Heavy Engineering</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>SQL Server</t>
-        </is>
-      </c>
-      <c r="C71" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Flask Framework</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Agile methodology</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>PostgreSQL</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Microservices</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Excel</t>
-        </is>
-      </c>
-      <c r="C76" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Front End</t>
-        </is>
-      </c>
-      <c r="C77" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>PHP</t>
-        </is>
-      </c>
-      <c r="C78" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>React.js</t>
-        </is>
-      </c>
-      <c r="C79" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Data Pipeline</t>
-        </is>
-      </c>
-      <c r="C80" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>